<commit_message>
aspen cover initial graph and loading in trees
</commit_message>
<xml_diff>
--- a/data/raw/aspen_meadow.xlsx
+++ b/data/raw/aspen_meadow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9E9C39-0890-4D67-ABEE-22212A62B218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141140F7-940A-4AC9-A78A-EE6C2C17E8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Ground Cover" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12407383-9CC2-42EA-B9EF-9C9CECC58899}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>